<commit_message>
Empreintes des composants r Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/Composants/Commande Farnell 2.xlsx
+++ b/Composants/Commande Farnell 2.xlsx
@@ -407,9 +407,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -427,9 +424,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -444,9 +438,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -455,6 +446,15 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:I15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +833,7 @@
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:12" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
@@ -843,15 +843,15 @@
       <c r="C10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>21</v>
       </c>
       <c r="I10" s="12" t="s">
@@ -863,170 +863,170 @@
       <c r="K10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22">
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20">
         <v>4.5100000000000001E-2</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="21">
         <v>2</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J11" s="22">
         <f>H11*I11</f>
         <v>9.0200000000000002E-2</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11" s="23">
         <f>0.2*J11</f>
         <v>1.804E-2</v>
       </c>
-      <c r="L11" s="25">
+      <c r="L11" s="23">
         <f>K11+J11</f>
         <v>0.10824</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17">
         <v>1754222</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22">
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20">
         <v>0.20699999999999999</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="21">
         <v>5</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="22">
         <f t="shared" ref="J12:J14" si="0">H12*I12</f>
         <v>1.0349999999999999</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="23">
         <f t="shared" ref="K12:K14" si="1">0.2*J12</f>
         <v>0.20699999999999999</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="23">
         <f t="shared" ref="L12:L14" si="2">K12+J12</f>
         <v>1.242</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17">
         <v>2326128</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22">
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20">
         <v>0.16</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="21">
         <v>2</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="22">
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="23">
         <f t="shared" si="1"/>
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="23">
         <f t="shared" si="2"/>
         <v>0.38400000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="24">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27">
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="24">
         <f>SUM(J11:J13)</f>
         <v>1.4452</v>
       </c>
-      <c r="K15" s="28">
+      <c r="K15" s="25">
         <f>J15*0.2</f>
         <v>0.28904000000000002</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="26">
         <f>J15+K15</f>
         <v>1.73424</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="28">
         <f ca="1">TODAY()</f>
-        <v>42059</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="I17" s="30"/>
+        <v>42066</v>
+      </c>
+      <c r="C17" s="27"/>
+      <c r="I17" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A15:I15"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>